<commit_message>
* Fix export header
* Clear header variable before add new.
</commit_message>
<xml_diff>
--- a/export/TestImportTrade_2.xlsx
+++ b/export/TestImportTrade_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="4995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AUTO-TAGGING" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="122">
   <si>
     <t>MisMatch</t>
   </si>
@@ -117,64 +117,70 @@
     <t>FC</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>PTF3</t>
+  </si>
+  <si>
+    <t>SEC3</t>
+  </si>
+  <si>
+    <t>12435</t>
+  </si>
+  <si>
+    <t>FUT</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>BD1</t>
+  </si>
+  <si>
+    <t>12383</t>
+  </si>
+  <si>
+    <t>PORTFOLIO</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>12355</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>TRN_FMLY</t>
+  </si>
+  <si>
+    <t>PTF1</t>
+  </si>
+  <si>
+    <t>FUT1</t>
+  </si>
+  <si>
+    <t>12353</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>SETTLE</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>PTF3</t>
-  </si>
-  <si>
-    <t>SEC3</t>
-  </si>
-  <si>
-    <t>12435</t>
-  </si>
-  <si>
-    <t>FUT</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>BD1</t>
-  </si>
-  <si>
-    <t>12383</t>
-  </si>
-  <si>
-    <t>PORTFOLIO</t>
-  </si>
-  <si>
-    <t>12355</t>
-  </si>
-  <si>
-    <t>COM</t>
-  </si>
-  <si>
-    <t>TRN_FMLY</t>
-  </si>
-  <si>
-    <t>PTF1</t>
-  </si>
-  <si>
-    <t>FUT1</t>
-  </si>
-  <si>
-    <t>12353</t>
-  </si>
-  <si>
-    <t>Bond</t>
-  </si>
-  <si>
-    <t>SETTLE</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>CUR</t>
@@ -829,7 +835,7 @@
   <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +936,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
@@ -956,54 +962,54 @@
       <c r="I3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J3">
-        <v>1</v>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4">
-        <v>2</v>
+      <c r="J4" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>28</v>
@@ -1015,45 +1021,45 @@
         <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J5">
-        <v>3</v>
+      <c r="J5" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J6">
-        <v>1</v>
+      <c r="J6" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1061,34 +1067,34 @@
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1096,214 +1102,226 @@
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
+        <v>53</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="T12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1311,28 +1329,28 @@
         <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1343,25 +1361,25 @@
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1372,25 +1390,25 @@
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1398,28 +1416,28 @@
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1430,25 +1448,25 @@
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1459,25 +1477,25 @@
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1488,13 +1506,13 @@
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>29</v>
@@ -1503,10 +1521,10 @@
         <v>30</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1514,28 +1532,28 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1543,28 +1561,28 @@
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1575,16 +1593,16 @@
         <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>30</v>
@@ -1593,7 +1611,7 @@
         <v>31</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1601,13 +1619,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>28</v>
@@ -1619,10 +1637,10 @@
         <v>30</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1630,28 +1648,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1659,28 +1677,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,16 +1706,16 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>29</v>
@@ -1706,10 +1724,10 @@
         <v>30</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,28 +1735,28 @@
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F29" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,28 +1764,28 @@
         <v>24</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1775,28 +1793,28 @@
         <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1807,10 +1825,10 @@
         <v>25</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>28</v>
@@ -1822,10 +1840,10 @@
         <v>30</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1833,28 +1851,28 @@
         <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1865,13 +1883,13 @@
         <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>29</v>
@@ -1880,10 +1898,10 @@
         <v>30</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1891,16 +1909,16 @@
         <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>29</v>
@@ -1909,10 +1927,10 @@
         <v>30</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1923,13 +1941,13 @@
         <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>29</v>
@@ -1938,10 +1956,10 @@
         <v>30</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1952,10 +1970,10 @@
         <v>25</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>28</v>
@@ -1967,10 +1985,10 @@
         <v>30</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1978,28 +1996,28 @@
         <v>24</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2007,28 +2025,28 @@
         <v>24</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2039,13 +2057,13 @@
         <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>29</v>
@@ -2054,10 +2072,10 @@
         <v>30</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2068,10 +2086,10 @@
         <v>25</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>28</v>
@@ -2083,10 +2101,10 @@
         <v>30</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2094,28 +2112,28 @@
         <v>24</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2126,25 +2144,25 @@
         <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2152,28 +2170,28 @@
         <v>24</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2181,28 +2199,28 @@
         <v>24</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2210,28 +2228,28 @@
         <v>24</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2239,28 +2257,28 @@
         <v>24</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2271,25 +2289,25 @@
         <v>25</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2297,28 +2315,28 @@
         <v>24</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2326,28 +2344,28 @@
         <v>24</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2355,28 +2373,28 @@
         <v>24</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2384,28 +2402,28 @@
         <v>24</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2416,25 +2434,25 @@
         <v>25</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2442,28 +2460,28 @@
         <v>24</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2471,13 +2489,13 @@
         <v>24</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>28</v>
@@ -2489,10 +2507,10 @@
         <v>30</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2506,22 +2524,22 @@
         <v>26</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2529,16 +2547,16 @@
         <v>24</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>29</v>
@@ -2547,10 +2565,10 @@
         <v>30</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2561,13 +2579,13 @@
         <v>25</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>29</v>
@@ -2579,7 +2597,7 @@
         <v>31</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2590,25 +2608,25 @@
         <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>